<commit_message>
Adding new graph into Excel
</commit_message>
<xml_diff>
--- a/hs/KernelPerceptron/KP_Performance_Results.xlsx
+++ b/hs/KernelPerceptron/KP_Performance_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\KernelPerceptron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F57FF7-E2D1-4A89-A580-18AE74344F4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EE4B3E-433F-4A2B-9068-AF0CB42E0350}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GenError" sheetId="1" r:id="rId1"/>
@@ -811,9 +811,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -852,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -860,6 +861,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2641,6 +2643,561 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Budget Kernel Perceptron</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:shade val="76000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>GenError!$G$61:$G$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6999999999999913E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.19999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7000000000000024E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9000000000000017E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7000000000000015E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4000000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1000000000000019E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1000000000000019E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5000000000000022E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0000000000000027E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0000000000000044E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.699999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3000000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.3000000000000029E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6393-43B1-85CB-49E1B6D3096E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Description Kernel Perceptron</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:tint val="77000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>GenError!$J$61:$J$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.0000000000000018E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7000000000000015E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.000000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5000000000000013E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2999999999999927E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4999999999999902E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.599999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5000000000000022E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0000000000000018E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4999999999999911E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0000000000000036E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7999999999999932E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.4999999999999929E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.0000000000000062E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.5000000000000022E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6393-43B1-85CB-49E1B6D3096E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="430204144"/>
+        <c:axId val="430205456"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="430204144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Trial Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430205456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="430205456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Generalization</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Error</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430204144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
@@ -3351,7 +3908,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4109,7 +4666,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4707,6 +5264,12 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
   <a:schemeClr val="dk1"/>
   <cs:variation>
@@ -4733,7 +5296,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
 </cs:colorStyle>
@@ -6249,6 +6812,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6784,6 +7850,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B450601-605C-46C8-AA20-774768BCA87A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7170,8 +8272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8996,8 +10098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D4E763-7B26-4572-B2E3-B397149B68CA}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10248,8 +11350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAB718F-DF94-4DDA-BA48-1B1D5687EE31}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10686,8 +11788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B9939-293C-4DC9-8D3A-5A6F24858279}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10801,7 +11903,7 @@
         <f>_xlfn.STDEV.S(B2:F2)</f>
         <v>3.6195069139317853</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="7">
         <f>_xlfn.CONFIDENCE.NORM(0.05, H2, 5)</f>
         <v>3.1725793958339898</v>
       </c>
@@ -10833,7 +11935,7 @@
         <f>_xlfn.STDEV.S(K2:O2)</f>
         <v>6.2731172474297242E-2</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="7">
         <f>_xlfn.CONFIDENCE.NORM(0.05, Q2, 5)</f>
         <v>5.4985286670518725E-2</v>
       </c>
@@ -10864,7 +11966,7 @@
         <f>_xlfn.STDEV.S(T2:X2)</f>
         <v>6.3959362098132536E-2</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="7">
         <f>_xlfn.CONFIDENCE.NORM(0.05,Z2,5)</f>
         <v>5.6061822559912634E-2</v>
       </c>
@@ -10900,7 +12002,7 @@
         <f t="shared" ref="H3:H25" si="1">_xlfn.STDEV.S(B3:F3)</f>
         <v>2.7901305166604735</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="7">
         <f t="shared" ref="I3:I25" si="2">_xlfn.CONFIDENCE.NORM(0.05, H3, 5)</f>
         <v>2.4456122890034879</v>
       </c>
@@ -10932,7 +12034,7 @@
         <f t="shared" ref="Q3:Q25" si="4">_xlfn.STDEV.S(K3:O3)</f>
         <v>5.837208236820042E-2</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="7">
         <f t="shared" ref="R3:R25" si="5">_xlfn.CONFIDENCE.NORM(0.05, Q3, 5)</f>
         <v>5.1164445936120496E-2</v>
       </c>
@@ -10964,7 +12066,7 @@
         <f t="shared" ref="Z3:Z25" si="7">_xlfn.STDEV.S(T3:X3)</f>
         <v>6.2735157607198E-2</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="7">
         <f t="shared" ref="AA3:AA25" si="8">_xlfn.CONFIDENCE.NORM(0.05,Z3,5)</f>
         <v>5.4988779729333435E-2</v>
       </c>
@@ -11000,7 +12102,7 @@
         <f t="shared" si="1"/>
         <v>3.1730448783463503</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="7">
         <f t="shared" si="2"/>
         <v>2.7812453581316521</v>
       </c>
@@ -11032,7 +12134,7 @@
         <f t="shared" si="4"/>
         <v>5.9841457201508498E-2</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="7">
         <f t="shared" si="5"/>
         <v>5.2452386098070986E-2</v>
       </c>
@@ -11064,7 +12166,7 @@
         <f t="shared" si="7"/>
         <v>6.3076937148216189E-2</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="7">
         <f t="shared" si="8"/>
         <v>5.5288357200943793E-2</v>
       </c>
@@ -11100,7 +12202,7 @@
         <f t="shared" si="1"/>
         <v>2.9999626331006262</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="7">
         <f t="shared" si="2"/>
         <v>2.6295348688001714</v>
       </c>
@@ -11132,7 +12234,7 @@
         <f t="shared" si="4"/>
         <v>6.0039986675548315E-2</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="7">
         <f t="shared" si="5"/>
         <v>5.26264016570357E-2</v>
       </c>
@@ -11164,7 +12266,7 @@
         <f t="shared" si="7"/>
         <v>6.2076565626651925E-2</v>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="7">
         <f t="shared" si="8"/>
         <v>5.4411509013341824E-2</v>
       </c>
@@ -11200,7 +12302,7 @@
         <f t="shared" si="1"/>
         <v>3.3890328266335858</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="7">
         <f t="shared" si="2"/>
         <v>2.9705636632983032</v>
       </c>
@@ -11232,7 +12334,7 @@
         <f t="shared" si="4"/>
         <v>6.1050798520576176E-2</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="7">
         <f t="shared" si="5"/>
         <v>5.3512401023484424E-2</v>
       </c>
@@ -11264,7 +12366,7 @@
         <f t="shared" si="7"/>
         <v>6.3401892716227468E-2</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="7">
         <f t="shared" si="8"/>
         <v>5.5573188080991549E-2</v>
       </c>
@@ -11300,7 +12402,7 @@
         <f t="shared" si="1"/>
         <v>2.8087054847384798</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="7">
         <f t="shared" si="2"/>
         <v>2.4618936672143508</v>
       </c>
@@ -11332,7 +12434,7 @@
         <f t="shared" si="4"/>
         <v>6.3508267178376432E-2</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="7">
         <f t="shared" si="5"/>
         <v>5.5666427694806821E-2</v>
       </c>
@@ -11363,7 +12465,7 @@
         <f t="shared" si="7"/>
         <v>6.4639771039198643E-2</v>
       </c>
-      <c r="AA7">
+      <c r="AA7" s="7">
         <f t="shared" si="8"/>
         <v>5.6658216333566921E-2</v>
       </c>
@@ -11399,7 +12501,7 @@
         <f t="shared" si="1"/>
         <v>3.042485776466338</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="7">
         <f t="shared" si="2"/>
         <v>2.6668073624563875</v>
       </c>
@@ -11431,7 +12533,7 @@
         <f t="shared" si="4"/>
         <v>5.9036429431326524E-2</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="7">
         <f t="shared" si="5"/>
         <v>5.1746761111716381E-2</v>
       </c>
@@ -11463,7 +12565,7 @@
         <f t="shared" si="7"/>
         <v>6.1853051662792126E-2</v>
       </c>
-      <c r="AA8">
+      <c r="AA8" s="7">
         <f t="shared" si="8"/>
         <v>5.4215593985885088E-2</v>
       </c>
@@ -11499,7 +12601,7 @@
         <f t="shared" si="1"/>
         <v>3.5105471795718737</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="7">
         <f t="shared" si="2"/>
         <v>3.0770737326522908</v>
       </c>
@@ -11531,7 +12633,7 @@
         <f t="shared" si="4"/>
         <v>6.3061081500399491E-2</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="7">
         <f t="shared" si="5"/>
         <v>5.5274459368237015E-2</v>
       </c>
@@ -11562,7 +12664,7 @@
         <f t="shared" si="7"/>
         <v>6.2064482596731668E-2</v>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="7">
         <f t="shared" si="8"/>
         <v>5.4400917965258255E-2</v>
       </c>
@@ -11598,7 +12700,7 @@
         <f t="shared" si="1"/>
         <v>3.3373199277264294</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="7">
         <f t="shared" si="2"/>
         <v>2.9252361417676225</v>
       </c>
@@ -11630,7 +12732,7 @@
         <f t="shared" si="4"/>
         <v>6.2503599896325854E-2</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="7">
         <f t="shared" si="5"/>
         <v>5.4785814176309677E-2</v>
       </c>
@@ -11661,7 +12763,7 @@
         <f t="shared" si="7"/>
         <v>6.3405835693569848E-2</v>
       </c>
-      <c r="AA10">
+      <c r="AA10" s="7">
         <f t="shared" si="8"/>
         <v>5.5576644189509125E-2</v>
       </c>
@@ -11697,7 +12799,7 @@
         <f t="shared" si="1"/>
         <v>3.3421892076900717</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="7">
         <f t="shared" si="2"/>
         <v>2.9295041754121329</v>
       </c>
@@ -11729,7 +12831,7 @@
         <f t="shared" si="4"/>
         <v>6.0833378995416437E-2</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="7">
         <f t="shared" si="5"/>
         <v>5.3321827908920448E-2</v>
       </c>
@@ -11760,7 +12862,7 @@
         <f t="shared" si="7"/>
         <v>6.2202893823358217E-2</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="7">
         <f t="shared" si="8"/>
         <v>5.4522238525265283E-2</v>
       </c>
@@ -11796,7 +12898,7 @@
         <f t="shared" si="1"/>
         <v>2.9499516606208998</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="7">
         <f t="shared" si="2"/>
         <v>2.585699124145536</v>
       </c>
@@ -11828,7 +12930,7 @@
         <f t="shared" si="4"/>
         <v>6.0833378995416437E-2</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="7">
         <f t="shared" si="5"/>
         <v>5.3321827908920448E-2</v>
       </c>
@@ -11860,7 +12962,7 @@
         <f t="shared" si="7"/>
         <v>6.1973381382654943E-2</v>
       </c>
-      <c r="AA12">
+      <c r="AA12" s="7">
         <f t="shared" si="8"/>
         <v>5.4321065697646116E-2</v>
       </c>
@@ -11896,7 +12998,7 @@
         <f t="shared" si="1"/>
         <v>3.5396294015051897</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="7">
         <f t="shared" si="2"/>
         <v>3.1025649557068928</v>
       </c>
@@ -11928,7 +13030,7 @@
         <f t="shared" si="4"/>
         <v>5.9492016271092775E-2</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="7">
         <f t="shared" si="5"/>
         <v>5.2146093245961547E-2</v>
       </c>
@@ -11958,7 +13060,7 @@
         <f t="shared" si="7"/>
         <v>6.3174361888348088E-2</v>
       </c>
-      <c r="AA13">
+      <c r="AA13" s="7">
         <f t="shared" si="8"/>
         <v>5.5373752181679219E-2</v>
       </c>
@@ -11994,7 +13096,7 @@
         <f t="shared" si="1"/>
         <v>3.7533509961100044</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="7">
         <f t="shared" si="2"/>
         <v>3.2898967507859833</v>
       </c>
@@ -12026,7 +13128,7 @@
         <f t="shared" si="4"/>
         <v>6.0825159268184638E-2</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="7">
         <f t="shared" si="5"/>
         <v>5.3314623132724386E-2</v>
       </c>
@@ -12057,7 +13159,7 @@
         <f t="shared" si="7"/>
         <v>6.4429806766744174E-2</v>
       </c>
-      <c r="AA14">
+      <c r="AA14" s="7">
         <f t="shared" si="8"/>
         <v>5.6474177916044817E-2</v>
       </c>
@@ -12093,7 +13195,7 @@
         <f t="shared" si="1"/>
         <v>3.9002986680509499</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="7">
         <f t="shared" si="2"/>
         <v>3.4186996975274746</v>
       </c>
@@ -12125,7 +13227,7 @@
         <f t="shared" si="4"/>
         <v>5.9626336463009223E-2</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="7">
         <f t="shared" si="5"/>
         <v>5.2263827921830888E-2</v>
       </c>
@@ -12155,7 +13257,7 @@
         <f t="shared" si="7"/>
         <v>6.072314221118659E-2</v>
       </c>
-      <c r="AA15">
+      <c r="AA15" s="7">
         <f t="shared" si="8"/>
         <v>5.3225202882742316E-2</v>
       </c>
@@ -12191,7 +13293,7 @@
         <f t="shared" si="1"/>
         <v>4.7800212551828745</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="7">
         <f t="shared" si="2"/>
         <v>4.1897963746029525</v>
       </c>
@@ -12223,7 +13325,7 @@
         <f t="shared" si="4"/>
         <v>6.1422308650847843E-2</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="7">
         <f t="shared" si="5"/>
         <v>5.3838038026720075E-2</v>
       </c>
@@ -12255,7 +13357,7 @@
         <f t="shared" si="7"/>
         <v>6.262188115986303E-2</v>
       </c>
-      <c r="AA16">
+      <c r="AA16" s="7">
         <f t="shared" si="8"/>
         <v>5.48894903699279E-2</v>
       </c>
@@ -12291,7 +13393,7 @@
         <f t="shared" si="1"/>
         <v>4.2876272925710319</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="7">
         <f t="shared" si="2"/>
         <v>3.7582019675298497</v>
       </c>
@@ -12323,7 +13425,7 @@
         <f t="shared" si="4"/>
         <v>5.9686681931566808E-2</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="7">
         <f t="shared" si="5"/>
         <v>5.2316722085243274E-2</v>
       </c>
@@ -12355,7 +13457,7 @@
         <f t="shared" si="7"/>
         <v>6.3737743919909898E-2</v>
       </c>
-      <c r="AA17">
+      <c r="AA17" s="7">
         <f t="shared" si="8"/>
         <v>5.5867569231298972E-2</v>
       </c>
@@ -12391,7 +13493,7 @@
         <f t="shared" si="1"/>
         <v>4.3395763272467063</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="7">
         <f t="shared" si="2"/>
         <v>3.8037364673842728</v>
       </c>
@@ -12423,7 +13525,7 @@
         <f t="shared" si="4"/>
         <v>6.084159761216007E-2</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="7">
         <f t="shared" si="5"/>
         <v>5.332903171174861E-2</v>
       </c>
@@ -12455,7 +13557,7 @@
         <f t="shared" si="7"/>
         <v>6.307297360993841E-2</v>
       </c>
-      <c r="AA18">
+      <c r="AA18" s="7">
         <f t="shared" si="8"/>
         <v>5.5284883070302882E-2</v>
       </c>
@@ -12491,7 +13593,7 @@
         <f t="shared" si="1"/>
         <v>3.5303401394200038</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="7">
         <f t="shared" si="2"/>
         <v>3.0944227081039037</v>
       </c>
@@ -12523,7 +13625,7 @@
         <f t="shared" si="4"/>
         <v>6.1389738556211382E-2</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="7">
         <f t="shared" si="5"/>
         <v>5.3809489604622507E-2</v>
       </c>
@@ -12555,7 +13657,7 @@
         <f t="shared" si="7"/>
         <v>6.2182795048148283E-2</v>
       </c>
-      <c r="AA19">
+      <c r="AA19" s="7">
         <f t="shared" si="8"/>
         <v>5.4504621495755794E-2</v>
       </c>
@@ -12591,7 +13693,7 @@
         <f t="shared" si="1"/>
         <v>2.8742915127036053</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="7">
         <f t="shared" si="2"/>
         <v>2.5193812990726689</v>
       </c>
@@ -12623,7 +13725,7 @@
         <f t="shared" si="4"/>
         <v>6.1719526893844669E-2</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="7">
         <f t="shared" si="5"/>
         <v>5.4098556516177364E-2</v>
       </c>
@@ -12654,7 +13756,7 @@
         <f t="shared" si="7"/>
         <v>6.4410402886490248E-2</v>
       </c>
-      <c r="AA20">
+      <c r="AA20" s="7">
         <f t="shared" si="8"/>
         <v>5.6457169977627598E-2</v>
       </c>
@@ -12690,7 +13792,7 @@
         <f t="shared" si="1"/>
         <v>3.347385502149403</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="7">
         <f t="shared" si="2"/>
         <v>2.9340588446332099</v>
       </c>
@@ -12722,7 +13824,7 @@
         <f t="shared" si="4"/>
         <v>6.1046703432700009E-2</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="7">
         <f t="shared" si="5"/>
         <v>5.3508811586655318E-2</v>
       </c>
@@ -12754,7 +13856,7 @@
         <f t="shared" si="7"/>
         <v>6.2080592780675105E-2</v>
       </c>
-      <c r="AA21">
+      <c r="AA21" s="7">
         <f t="shared" si="8"/>
         <v>5.4415038904617512E-2</v>
       </c>
@@ -12790,7 +13892,7 @@
         <f t="shared" si="1"/>
         <v>3.8987177379235832E-3</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="7">
         <f t="shared" si="2"/>
         <v>3.4173139766357609E-3</v>
       </c>
@@ -12822,7 +13924,7 @@
         <f t="shared" si="4"/>
         <v>4.4721359549995798E-3</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="7">
         <f t="shared" si="5"/>
         <v>3.9199279690801071E-3</v>
       </c>
@@ -12854,7 +13956,7 @@
         <f t="shared" si="7"/>
         <v>4.9193495504995348E-3</v>
       </c>
-      <c r="AA22">
+      <c r="AA22" s="7">
         <f t="shared" si="8"/>
         <v>4.3119207659881153E-3</v>
       </c>
@@ -12890,7 +13992,7 @@
         <f t="shared" si="1"/>
         <v>6.4187226143524916E-3</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="7">
         <f t="shared" si="2"/>
         <v>5.6261550531886018E-3</v>
       </c>
@@ -12922,7 +14024,7 @@
         <f t="shared" si="4"/>
         <v>5.2725705305856291E-3</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="7">
         <f t="shared" si="5"/>
         <v>4.6215269168381288E-3</v>
       </c>
@@ -12954,7 +14056,7 @@
         <f t="shared" si="7"/>
         <v>5.7183913821983196E-3</v>
       </c>
-      <c r="AA23">
+      <c r="AA23" s="7">
         <f t="shared" si="8"/>
         <v>5.0122989423357E-3</v>
       </c>
@@ -12990,7 +14092,7 @@
         <f t="shared" si="1"/>
         <v>1.7052611823412236</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="7">
         <f t="shared" si="2"/>
         <v>1.4946998638923541</v>
       </c>
@@ -13022,7 +14124,7 @@
         <f t="shared" si="4"/>
         <v>2.3593157270700313</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="7">
         <f t="shared" si="5"/>
         <v>2.0679934151137078</v>
       </c>
@@ -13054,7 +14156,7 @@
         <f t="shared" si="7"/>
         <v>1.466097609301642</v>
       </c>
-      <c r="AA24">
+      <c r="AA24" s="7">
         <f t="shared" si="8"/>
         <v>1.2850676012383273</v>
       </c>
@@ -13090,7 +14192,7 @@
         <f t="shared" si="1"/>
         <v>7.3459453442018674</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="7">
         <f t="shared" si="2"/>
         <v>6.43888667603653</v>
       </c>
@@ -13122,7 +14224,7 @@
         <f t="shared" si="4"/>
         <v>4.6582760008397903</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="7">
         <f t="shared" si="5"/>
         <v>4.0830839149630096</v>
       </c>
@@ -13153,14 +14255,14 @@
         <f t="shared" si="7"/>
         <v>3.5162429239175155</v>
       </c>
-      <c r="AA25">
+      <c r="AA25" s="7">
         <f t="shared" si="8"/>
         <v>3.0820661809566072</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D23 K19:K20 L11 M4 M9 M13 N18 N5 N16 O15 M2 U5:V5 U13 U16:U17 V8 V14 V16:W16 V18:V19 V20 W12 V2:V3" formula="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Adding spreadsheet with Python Budget timing results
</commit_message>
<xml_diff>
--- a/hs/KernelPerceptron/KP_Performance_Results.xlsx
+++ b/hs/KernelPerceptron/KP_Performance_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\KernelPerceptron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EE4B3E-433F-4A2B-9068-AF0CB42E0350}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9C268B-1A5A-4B7F-A09E-748757B3BB61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="273">
   <si>
     <t>Data File Index</t>
   </si>
@@ -805,6 +805,54 @@
   </si>
   <si>
     <t>KPD_CI</t>
+  </si>
+  <si>
+    <t>PyB_1</t>
+  </si>
+  <si>
+    <t>PyB_2</t>
+  </si>
+  <si>
+    <t>PyB_3</t>
+  </si>
+  <si>
+    <t>PyB_4</t>
+  </si>
+  <si>
+    <t>PyB_5</t>
+  </si>
+  <si>
+    <t>PyB_Ave</t>
+  </si>
+  <si>
+    <t>PyB_STD</t>
+  </si>
+  <si>
+    <t>PyB_CI</t>
+  </si>
+  <si>
+    <t>PyBN_1</t>
+  </si>
+  <si>
+    <t>PyBN_2</t>
+  </si>
+  <si>
+    <t>PyBN_3</t>
+  </si>
+  <si>
+    <t>PyBN_4</t>
+  </si>
+  <si>
+    <t>PyBN_5</t>
+  </si>
+  <si>
+    <t>PyBN_Ave</t>
+  </si>
+  <si>
+    <t>PyBN_STD</t>
+  </si>
+  <si>
+    <t>PyBN_CI</t>
   </si>
 </sst>
 </file>
@@ -816,7 +864,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -828,6 +876,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2873,7 +2927,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -5251,6 +5304,682 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Haskel KPB</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>TimingCalc!$P$2:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.3498</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34360000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34680000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34820000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.34860000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.34920000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.34440000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.34620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.35799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.34920000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34920000000000007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.34760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.3498</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2F23-4FF0-8904-EECBE1B1AA0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Naive Python KPB</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>TimingCalc!$G$28:$G$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82159999999999989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81980000000000008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82159999999999989</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82199999999999984</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8206</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82479999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82319999999999993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.82199999999999984</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8206</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82319999999999993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.81899999999999973</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.82340000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.82360000000000011</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.82079999999999986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.81799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.81899999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2F23-4FF0-8904-EECBE1B1AA0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Numpy Python KPB</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>TimingCalc!$P$28:$P$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.42659999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40240000000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40879999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42359999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.41920000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41459999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.42099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.41879999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.43260000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.39600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41360000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.41039999999999993</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.4204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.42399999999999993</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.42259999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.42219999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2F23-4FF0-8904-EECBE1B1AA0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="330615880"/>
+        <c:axId val="330618176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="330615880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Trial</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Index</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="330618176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="330618176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (Seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="330615880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
@@ -5302,6 +6031,33 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -7315,6 +8071,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7999,6 +9258,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E9C285D-9DC1-4D20-9CBD-1382F19BD2CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8272,8 +9572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11351,7 +12651,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11786,10 +13086,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B9939-293C-4DC9-8D3A-5A6F24858279}">
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14260,11 +15560,1244 @@
         <v>3.0820661809566072</v>
       </c>
     </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="C28">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="D28">
+        <v>0.82</v>
+      </c>
+      <c r="E28">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="F28">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="G28">
+        <f>AVERAGE(B28:F28)</f>
+        <v>0.82</v>
+      </c>
+      <c r="H28">
+        <f>_xlfn.STDEV.S(B28:F28)</f>
+        <v>1.5811388300841912E-3</v>
+      </c>
+      <c r="I28" s="7">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, H28, 5)</f>
+        <v>1.3859038243496788E-3</v>
+      </c>
+      <c r="K28">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L28">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="M28">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="N28">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="O28">
+        <v>0.433</v>
+      </c>
+      <c r="P28">
+        <f>AVERAGE(K28:O28)</f>
+        <v>0.42659999999999998</v>
+      </c>
+      <c r="Q28">
+        <f>_xlfn.STDEV.S(K28:O28)</f>
+        <v>4.3358966777357639E-3</v>
+      </c>
+      <c r="R28" s="7">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, Q28, 5)</f>
+        <v>3.8005111716465103E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>0.82</v>
+      </c>
+      <c r="C29">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="D29">
+        <v>0.82</v>
+      </c>
+      <c r="E29">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="F29">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G47" si="9">AVERAGE(B29:F29)</f>
+        <v>0.82159999999999989</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:H47" si="10">_xlfn.STDEV.S(B29:F29)</f>
+        <v>2.5099800796022287E-3</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" ref="I29:I47" si="11">_xlfn.CONFIDENCE.NORM(0.05, H29, 5)</f>
+        <v>2.2000541161695552E-3</v>
+      </c>
+      <c r="K29">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="L29">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="M29">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="N29">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="O29">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="P29">
+        <f t="shared" ref="P29:P47" si="12">AVERAGE(K29:O29)</f>
+        <v>0.40240000000000009</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" ref="Q29:Q47" si="13">_xlfn.STDEV.S(K29:O29)</f>
+        <v>8.9442719099991667E-4</v>
+      </c>
+      <c r="R29" s="7">
+        <f t="shared" ref="R29:R47" si="14">_xlfn.CONFIDENCE.NORM(0.05, Q29, 5)</f>
+        <v>7.8398559381602213E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="C30">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="D30">
+        <v>0.82</v>
+      </c>
+      <c r="E30">
+        <v>0.82</v>
+      </c>
+      <c r="F30">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="G30">
+        <f>AVERAGE(B30:F30)</f>
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="10"/>
+        <v>1.2247448713915902E-3</v>
+      </c>
+      <c r="I30" s="7">
+        <f t="shared" si="11"/>
+        <v>1.073516486230295E-3</v>
+      </c>
+      <c r="K30">
+        <v>0.41</v>
+      </c>
+      <c r="L30">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="M30">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="N30">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="O30">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="12"/>
+        <v>0.40879999999999994</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="13"/>
+        <v>8.366600265340764E-4</v>
+      </c>
+      <c r="R30" s="7">
+        <f t="shared" si="14"/>
+        <v>7.3335137205651855E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="C31">
+        <v>0.82</v>
+      </c>
+      <c r="D31">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="E31">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="F31">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="9"/>
+        <v>0.81980000000000008</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="10"/>
+        <v>1.9235384061671362E-3</v>
+      </c>
+      <c r="I31" s="7">
+        <f t="shared" si="11"/>
+        <v>1.6860247706702461E-3</v>
+      </c>
+      <c r="K31">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L31">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="M31">
+        <v>0.42</v>
+      </c>
+      <c r="N31">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="O31">
+        <v>0.42</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="12"/>
+        <v>0.42080000000000001</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="13"/>
+        <v>8.3666002653407629E-4</v>
+      </c>
+      <c r="R31" s="7">
+        <f t="shared" si="14"/>
+        <v>7.3335137205651844E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="C32">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="D32">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="E32">
+        <v>0.82</v>
+      </c>
+      <c r="F32">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="9"/>
+        <v>0.82159999999999989</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="10"/>
+        <v>3.1304951684997086E-3</v>
+      </c>
+      <c r="I32" s="7">
+        <f t="shared" si="11"/>
+        <v>2.7439495783560777E-3</v>
+      </c>
+      <c r="K32">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="L32">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="M32">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="N32">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="O32">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="12"/>
+        <v>0.42359999999999998</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="13"/>
+        <v>5.4772255750516654E-4</v>
+      </c>
+      <c r="R32" s="7">
+        <f t="shared" si="14"/>
+        <v>4.8009116763553125E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="C33">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="D33">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="E33">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="F33">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="9"/>
+        <v>0.82199999999999984</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="10"/>
+        <v>1.22474487139159E-3</v>
+      </c>
+      <c r="I33" s="7">
+        <f t="shared" si="11"/>
+        <v>1.0735164862302948E-3</v>
+      </c>
+      <c r="K33">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L33">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="M33">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="N33">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="O33">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="12"/>
+        <v>0.42180000000000001</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="13"/>
+        <v>8.3666002653407629E-4</v>
+      </c>
+      <c r="R33" s="7">
+        <f t="shared" si="14"/>
+        <v>7.3335137205651844E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>0.82</v>
+      </c>
+      <c r="C34">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="D34">
+        <v>0.82</v>
+      </c>
+      <c r="E34">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="F34">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="9"/>
+        <v>0.8206</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="10"/>
+        <v>1.3416407864998751E-3</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" si="11"/>
+        <v>1.175978390724033E-3</v>
+      </c>
+      <c r="K34">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L34">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="M34">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="N34">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="O34">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="12"/>
+        <v>0.42180000000000001</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="13"/>
+        <v>1.3038404810405309E-3</v>
+      </c>
+      <c r="R34" s="7">
+        <f t="shared" si="14"/>
+        <v>1.1428455709482381E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="C35">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="D35">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="E35">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="F35">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="9"/>
+        <v>0.82479999999999998</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="10"/>
+        <v>2.3874672772626667E-3</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" si="11"/>
+        <v>2.0926688834097258E-3</v>
+      </c>
+      <c r="K35">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="L35">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="M35">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="N35">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="O35">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="12"/>
+        <v>0.41920000000000002</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="13"/>
+        <v>2.7748873851023243E-3</v>
+      </c>
+      <c r="R35" s="7">
+        <f t="shared" si="14"/>
+        <v>2.4322513406037955E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="C36">
+        <v>0.82</v>
+      </c>
+      <c r="D36">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="E36">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="F36">
+        <v>0.82</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="9"/>
+        <v>0.82</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="10"/>
+        <v>1.2247448713915902E-3</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" si="11"/>
+        <v>1.073516486230295E-3</v>
+      </c>
+      <c r="K36">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="L36">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="M36">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="N36">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="O36">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="12"/>
+        <v>0.41459999999999997</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="13"/>
+        <v>8.9442719099991667E-4</v>
+      </c>
+      <c r="R36" s="7">
+        <f t="shared" si="14"/>
+        <v>7.8398559381602213E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="C37">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D37">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="E37">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="F37">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="9"/>
+        <v>0.82319999999999993</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="10"/>
+        <v>1.7888543819998333E-3</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="11"/>
+        <v>1.5679711876320443E-3</v>
+      </c>
+      <c r="K37">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="L37">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="M37">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="N37">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="O37">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="12"/>
+        <v>0.41839999999999999</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="13"/>
+        <v>5.4772255750516654E-4</v>
+      </c>
+      <c r="R37" s="7">
+        <f t="shared" si="14"/>
+        <v>4.8009116763553125E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="C38">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D38">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="E38">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="F38">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="9"/>
+        <v>0.82199999999999984</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="10"/>
+        <v>2.236067977499792E-3</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="11"/>
+        <v>1.9599639845400557E-3</v>
+      </c>
+      <c r="K38">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="L38">
+        <v>0.42</v>
+      </c>
+      <c r="M38">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="N38">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="O38">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="12"/>
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="13"/>
+        <v>7.0710678118654816E-4</v>
+      </c>
+      <c r="R38" s="7">
+        <f t="shared" si="14"/>
+        <v>6.1979503230456194E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="C39">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="D39">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="E39">
+        <v>0.82</v>
+      </c>
+      <c r="F39">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="9"/>
+        <v>0.8206</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="10"/>
+        <v>1.6733200530681526E-3</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="11"/>
+        <v>1.4667027441130369E-3</v>
+      </c>
+      <c r="K39">
+        <v>0.42</v>
+      </c>
+      <c r="L39">
+        <v>0.42</v>
+      </c>
+      <c r="M39">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="N39">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="O39">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="12"/>
+        <v>0.41879999999999995</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="13"/>
+        <v>1.3038404810405309E-3</v>
+      </c>
+      <c r="R39" s="7">
+        <f t="shared" si="14"/>
+        <v>1.1428455709482381E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="C40">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="D40">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="E40">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="F40">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="9"/>
+        <v>0.82319999999999993</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="10"/>
+        <v>3.3466401061363052E-3</v>
+      </c>
+      <c r="I40" s="7">
+        <f t="shared" si="11"/>
+        <v>2.9334054882260738E-3</v>
+      </c>
+      <c r="K40">
+        <v>0.433</v>
+      </c>
+      <c r="L40">
+        <v>0.433</v>
+      </c>
+      <c r="M40">
+        <v>0.432</v>
+      </c>
+      <c r="N40">
+        <v>0.433</v>
+      </c>
+      <c r="O40">
+        <v>0.432</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="12"/>
+        <v>0.43260000000000004</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="13"/>
+        <v>5.4772255750516654E-4</v>
+      </c>
+      <c r="R40" s="7">
+        <f t="shared" si="14"/>
+        <v>4.8009116763553125E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>14</v>
+      </c>
+      <c r="B41">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="C41">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="D41">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="E41">
+        <v>0.82</v>
+      </c>
+      <c r="F41">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="9"/>
+        <v>0.81899999999999973</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="10"/>
+        <v>1.8708286933869723E-3</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" si="11"/>
+        <v>1.639823519311115E-3</v>
+      </c>
+      <c r="K41">
+        <v>0.4</v>
+      </c>
+      <c r="L41">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="M41">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="N41">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="O41">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="12"/>
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="13"/>
+        <v>2.3452078799117166E-3</v>
+      </c>
+      <c r="R41" s="7">
+        <f t="shared" si="14"/>
+        <v>2.055627569080436E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="C42">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="D42">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="E42">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="F42">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="9"/>
+        <v>0.82340000000000002</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="10"/>
+        <v>2.3021728866442696E-3</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="11"/>
+        <v>2.0179064274479571E-3</v>
+      </c>
+      <c r="K42">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="L42">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="M42">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="N42">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="O42">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="12"/>
+        <v>0.41360000000000002</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="13"/>
+        <v>8.9442719099991667E-4</v>
+      </c>
+      <c r="R42" s="7">
+        <f t="shared" si="14"/>
+        <v>7.8398559381602213E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>16</v>
+      </c>
+      <c r="B43">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="C43">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="D43">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="E43">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="F43">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="9"/>
+        <v>0.82360000000000011</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="10"/>
+        <v>2.7018512172212617E-3</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="shared" si="11"/>
+        <v>2.3682334931787088E-3</v>
+      </c>
+      <c r="K43">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="L43">
+        <v>0.41</v>
+      </c>
+      <c r="M43">
+        <v>0.41</v>
+      </c>
+      <c r="N43">
+        <v>0.41</v>
+      </c>
+      <c r="O43">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="12"/>
+        <v>0.41039999999999993</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="13"/>
+        <v>5.4772255750516665E-4</v>
+      </c>
+      <c r="R43" s="7">
+        <f t="shared" si="14"/>
+        <v>4.8009116763553136E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>17</v>
+      </c>
+      <c r="B44">
+        <v>0.82</v>
+      </c>
+      <c r="C44">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="D44">
+        <v>0.82</v>
+      </c>
+      <c r="E44">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="F44">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="9"/>
+        <v>0.82079999999999986</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="10"/>
+        <v>8.366600265340764E-4</v>
+      </c>
+      <c r="I44" s="7">
+        <f t="shared" si="11"/>
+        <v>7.3335137205651855E-4</v>
+      </c>
+      <c r="K44">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="L44">
+        <v>0.42</v>
+      </c>
+      <c r="M44">
+        <v>0.42</v>
+      </c>
+      <c r="N44">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="O44">
+        <v>0.42</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="12"/>
+        <v>0.4204</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="13"/>
+        <v>1.5165750888103116E-3</v>
+      </c>
+      <c r="R44" s="7">
+        <f t="shared" si="14"/>
+        <v>1.3293122498191689E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>18</v>
+      </c>
+      <c r="B45">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="C45">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="D45">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="E45">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="F45">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="9"/>
+        <v>0.82</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="10"/>
+        <v>1.8708286933869726E-3</v>
+      </c>
+      <c r="I45" s="7">
+        <f t="shared" si="11"/>
+        <v>1.6398235193111153E-3</v>
+      </c>
+      <c r="K45">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="L45">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="M45">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="N45">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="O45">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="12"/>
+        <v>0.42399999999999993</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="13"/>
+        <v>7.0710678118654816E-4</v>
+      </c>
+      <c r="R45" s="7">
+        <f t="shared" si="14"/>
+        <v>6.1979503230456194E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>19</v>
+      </c>
+      <c r="B46">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="C46">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="D46">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="E46">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="F46">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="9"/>
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="10"/>
+        <v>2.1213203435596446E-3</v>
+      </c>
+      <c r="I46" s="7">
+        <f t="shared" si="11"/>
+        <v>1.8593850969136861E-3</v>
+      </c>
+      <c r="K46">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L46">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="M46">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="N46">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="O46">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="12"/>
+        <v>0.42259999999999998</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="13"/>
+        <v>5.4772255750516654E-4</v>
+      </c>
+      <c r="R46" s="7">
+        <f t="shared" si="14"/>
+        <v>4.8009116763553125E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="C47">
+        <v>0.82</v>
+      </c>
+      <c r="D47">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="E47">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="F47">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="9"/>
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="10"/>
+        <v>2.1213203435596446E-3</v>
+      </c>
+      <c r="I47" s="7">
+        <f t="shared" si="11"/>
+        <v>1.8593850969136861E-3</v>
+      </c>
+      <c r="K47">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="L47">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="M47">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="N47">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="O47">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="12"/>
+        <v>0.42219999999999996</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="13"/>
+        <v>8.3666002653407629E-4</v>
+      </c>
+      <c r="R47" s="7">
+        <f t="shared" si="14"/>
+        <v>7.3335137205651844E-4</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D23 K19:K20 L11 M4 M9 M13 N18 N5 N16 O15 M2 U5:V5 U13 U16:U17 V8 V14 V16:W16 V18:V19 V20 W12 V2:V3" formula="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>